<commit_message>
Got to modelling stage of homework
</commit_message>
<xml_diff>
--- a/Homework/Unit3/iowa-full-working/Iowa_Full_FieldReview.xlsx
+++ b/Homework/Unit3/iowa-full-working/Iowa_Full_FieldReview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4956c785816d6d1c/General-Assembly/my-1019-repo/Homework/Unit3/iowa-full-working/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="8_{02239267-7248-2A41-AB38-AA47D8ECEF6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF6583E6-6907-4D40-9F1D-68CA28F8D886}"/>
+  <xr:revisionPtr revIDLastSave="346" documentId="8_{02239267-7248-2A41-AB38-AA47D8ECEF6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{73E5B41E-ED41-3949-A62D-0F0E3F42F795}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="500" windowWidth="37000" windowHeight="21100" activeTab="3" xr2:uid="{C03783DD-5B06-D044-94ED-55443160CBB6}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="20820" windowHeight="21100" firstSheet="1" xr2:uid="{C03783DD-5B06-D044-94ED-55443160CBB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Review" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Field Review'!$A$1:$K$82</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="184">
   <si>
     <t>Id</t>
   </si>
@@ -493,33 +493,6 @@
     <t>During testing set verbose=1</t>
   </si>
   <si>
-    <t>{'col':'LotShape', mapping:{"Reg":0,"IR1":1,"IR2":2,"IR3":3}}</t>
-  </si>
-  <si>
-    <t>{'col':'Utilities', mapping:{"AllPub":0,"NoSwer":1,"NoSeWa":2,"ELO":3}}</t>
-  </si>
-  <si>
-    <t>{'col':'LotConfig', mapping:{'Gtl':1,'Mod':2,'Sev':3,}}</t>
-  </si>
-  <si>
-    <t>{'col':'LandSlope', mapping:{'Gtl':1,'Mod':2,'Sev':3,}}</t>
-  </si>
-  <si>
-    <t>{'col':'ExterQual', mapping:{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
-  </si>
-  <si>
-    <t>{'col':'ExterCond', mapping:{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
-  </si>
-  <si>
-    <t>{'col':'HeatingQC', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
-  </si>
-  <si>
-    <t>{'col':'KitchenQual', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
-  </si>
-  <si>
-    <t>{'col':'PavedDrive', mapping:{'Y':1,'P':2,'N':3}}</t>
-  </si>
-  <si>
     <t>]</t>
   </si>
   <si>
@@ -560,6 +533,69 @@
   </si>
   <si>
     <t>Review record, then decide, ended up select "Sbrkr"</t>
+  </si>
+  <si>
+    <t>Need to build a function that does this in order to ensure that only training data is used for this substitution.</t>
+  </si>
+  <si>
+    <t>Given 1360 are typical functionality maybe onehot split?</t>
+  </si>
+  <si>
+    <t>has_porch_flag; total_porch_sf (sum of porchSF values these)</t>
+  </si>
+  <si>
+    <t>Created function</t>
+  </si>
+  <si>
+    <t>{'col':'LotShape', 'mapping':{"Reg":0,"IR1":1,"IR2":2,"IR3":3}}</t>
+  </si>
+  <si>
+    <t>{'col':'Utilities', 'mapping':{"AllPub":0,"NoSwer":1,"NoSeWa":2,"ELO":3}}</t>
+  </si>
+  <si>
+    <t>{'col':'LotConfig', 'mapping':{'Gtl':1,'Mod':2,'Sev':3,}}</t>
+  </si>
+  <si>
+    <t>{'col':'LandSlope', 'mapping':{'Gtl':1,'Mod':2,'Sev':3,}}</t>
+  </si>
+  <si>
+    <t>{'col':'ExterQual', 'mapping':{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'ExterCond', 'mapping':{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'BsmtQual', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'BsmtCond', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'BsmtExposure', 'mapping':{'Gd':1,'Av':2,'Mn':3,'No':4,'NA':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'HeatingQC', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'KitchenQual', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'FireplaceQu', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'GarageFinish', 'mapping':{'Fin':1,'RFn':2,'Unf':3,'NA':4,}}</t>
+  </si>
+  <si>
+    <t>{'col':'GarageQual', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'GarageCond', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
+  </si>
+  <si>
+    <t>{'col':'PavedDrive', 'mapping':{'Y':1,'P':2,'N':3}}</t>
+  </si>
+  <si>
+    <t>{'col':'PoolQC', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}}</t>
   </si>
 </sst>
 </file>
@@ -958,11 +994,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC897A8-82EC-B640-BF1D-F20547F20C84}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A73" sqref="A73"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,7 +1111,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1122,7 +1158,7 @@
         <v>1369</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>99</v>
@@ -2486,10 +2522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583B48E7-93EF-1443-917E-8067A37EE097}">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2521,7 +2557,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4">
-        <f t="shared" ref="B4:B8" si="1">B3+1</f>
+        <f t="shared" ref="B4:B5" si="1">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -2532,69 +2568,60 @@
         <v>3. Create manual OneHotEncoding</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>4. Extract file for use in model pipeline (enables target encoding parameters to be manipulated)</v>
-      </c>
-    </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6">
-        <f t="shared" ref="B6:B9" si="2">B5+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>144</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>5. Design code for target_encoded columns</v>
+        <v>4. Design code for target_encoded columns</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" ref="B6:B9" si="2">B6+1</f>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>145</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>6. Design code for ordinal_encoded columns</v>
+        <v>5. Design code for ordinal_encoded columns</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>146</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>7. Design code for onehot encoded columns</v>
+        <v>6. Design code for onehot encoded columns</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>8. Run individual code sets and expected modelling data set (noting params in pipeline that may change)</v>
+        <v>7. Run individual code sets and expected modelling data set (noting params in pipeline that may change)</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2607,7 +2634,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2649,9 +2676,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -2665,13 +2692,15 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="4"/>
+        <v>156</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -2689,13 +2718,13 @@
         <v>99</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>25</v>
@@ -2717,7 +2746,7 @@
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>26</v>
@@ -2737,7 +2766,7 @@
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>30</v>
@@ -2764,7 +2793,7 @@
     </row>
     <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>31</v>
@@ -2791,7 +2820,7 @@
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>32</v>
@@ -2818,7 +2847,7 @@
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>33</v>
@@ -2840,7 +2869,7 @@
     </row>
     <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>35</v>
@@ -2862,7 +2891,7 @@
     </row>
     <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>42</v>
@@ -2878,13 +2907,13 @@
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>57</v>
@@ -2911,7 +2940,7 @@
     </row>
     <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>58</v>
@@ -2933,7 +2962,7 @@
     </row>
     <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>59</v>
@@ -2953,7 +2982,7 @@
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
@@ -2980,7 +3009,7 @@
     </row>
     <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>63</v>
@@ -3007,7 +3036,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>64</v>
@@ -3034,7 +3063,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>72</v>
@@ -3063,7 +3092,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>73</v>
@@ -3087,7 +3116,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>74</v>
@@ -3109,7 +3138,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3121,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF70325-4BF7-474E-97AC-D81BF0C0FC1C}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3158,7 +3187,7 @@
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -3180,7 +3209,7 @@
     </row>
     <row r="3" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>34</v>
@@ -3199,6 +3228,9 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
       <c r="B4" s="6" t="s">
         <v>55</v>
       </c>
@@ -3216,10 +3248,13 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
       <c r="B5" s="6" t="s">
         <v>66</v>
       </c>
@@ -3231,7 +3266,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -3269,12 +3304,158 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C540EFC9-8084-A04D-B11E-F633CB2BA266}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6">
+        <v>37</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3284,7 +3465,7 @@
   <dimension ref="D7:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3399,8 +3580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7558D544-BD0D-5D4D-90CD-3181838E1238}">
   <dimension ref="D5:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3410,10 +3591,10 @@
         <v>81</v>
       </c>
       <c r="M5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="P5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="4:16" x14ac:dyDescent="0.2">
@@ -3421,15 +3602,15 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="M6" t="str">
         <f>"'"&amp;D6&amp;"',"</f>
         <v>'LotShape',</v>
       </c>
       <c r="P6" t="str">
-        <f>E6&amp;","</f>
-        <v>{'col':'LotShape', mapping:{"Reg":0,"IR1":1,"IR2":2,"IR3":3}},</v>
+        <f t="shared" ref="P6:P22" si="0">E6&amp;","</f>
+        <v>{'col':'LotShape', 'mapping':{"Reg":0,"IR1":1,"IR2":2,"IR3":3}},</v>
       </c>
     </row>
     <row r="7" spans="4:16" x14ac:dyDescent="0.2">
@@ -3437,15 +3618,15 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" ref="M7:M23" si="0">"'"&amp;D7&amp;"',"</f>
+        <f t="shared" ref="M7:M22" si="1">"'"&amp;D7&amp;"',"</f>
         <v>'Utilities',</v>
       </c>
       <c r="P7" t="str">
-        <f>E7&amp;","</f>
-        <v>{'col':'Utilities', mapping:{"AllPub":0,"NoSwer":1,"NoSeWa":2,"ELO":3}},</v>
+        <f t="shared" si="0"/>
+        <v>{'col':'Utilities', 'mapping':{"AllPub":0,"NoSwer":1,"NoSeWa":2,"ELO":3}},</v>
       </c>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.2">
@@ -3453,15 +3634,15 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>'LotConfig',</v>
+      </c>
+      <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v>'LotConfig',</v>
-      </c>
-      <c r="P8" t="str">
-        <f>E8&amp;","</f>
-        <v>{'col':'LotConfig', mapping:{'Gtl':1,'Mod':2,'Sev':3,}},</v>
+        <v>{'col':'LotConfig', 'mapping':{'Gtl':1,'Mod':2,'Sev':3,}},</v>
       </c>
     </row>
     <row r="9" spans="4:16" x14ac:dyDescent="0.2">
@@ -3469,15 +3650,15 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>'LandSlope',</v>
+      </c>
+      <c r="P9" t="str">
         <f t="shared" si="0"/>
-        <v>'LandSlope',</v>
-      </c>
-      <c r="P9" t="str">
-        <f>E9&amp;","</f>
-        <v>{'col':'LandSlope', mapping:{'Gtl':1,'Mod':2,'Sev':3,}},</v>
+        <v>{'col':'LandSlope', 'mapping':{'Gtl':1,'Mod':2,'Sev':3,}},</v>
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.2">
@@ -3485,15 +3666,15 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>'ExterQual',</v>
+      </c>
+      <c r="P10" t="str">
         <f t="shared" si="0"/>
-        <v>'ExterQual',</v>
-      </c>
-      <c r="P10" t="str">
-        <f>E10&amp;","</f>
-        <v>{'col':'ExterQual', mapping:{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'ExterQual', 'mapping':{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.2">
@@ -3501,15 +3682,15 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>'ExterCond',</v>
+      </c>
+      <c r="P11" t="str">
         <f t="shared" si="0"/>
-        <v>'ExterCond',</v>
-      </c>
-      <c r="P11" t="str">
-        <f>E11&amp;","</f>
-        <v>{'col':'ExterCond', mapping:{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'ExterCond', 'mapping':{'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.2">
@@ -3517,15 +3698,15 @@
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>'BsmtQual',</v>
+      </c>
+      <c r="P12" t="str">
         <f t="shared" si="0"/>
-        <v>'BsmtQual',</v>
-      </c>
-      <c r="P12" t="str">
-        <f>E12&amp;","</f>
-        <v>{'col':'BsmtQual', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'BsmtQual', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.2">
@@ -3533,15 +3714,15 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>'BsmtCond',</v>
+      </c>
+      <c r="P13" t="str">
         <f t="shared" si="0"/>
-        <v>'BsmtCond',</v>
-      </c>
-      <c r="P13" t="str">
-        <f>E13&amp;","</f>
-        <v>{'col':'BsmtCond', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'BsmtCond', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.2">
@@ -3549,15 +3730,15 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>'BsmtExposure',</v>
+      </c>
+      <c r="P14" t="str">
         <f t="shared" si="0"/>
-        <v>'BsmtExposure',</v>
-      </c>
-      <c r="P14" t="str">
-        <f>E14&amp;","</f>
-        <v>{'col':'BsmtExposure', mapping:{'Gd':1,'Av':2,'Mn':3,'No':4,'NA':5,}},</v>
+        <v>{'col':'BsmtExposure', 'mapping':{'Gd':1,'Av':2,'Mn':3,'No':4,'NA':5,}},</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.2">
@@ -3565,15 +3746,15 @@
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>'HeatingQC',</v>
+      </c>
+      <c r="P15" t="str">
         <f t="shared" si="0"/>
-        <v>'HeatingQC',</v>
-      </c>
-      <c r="P15" t="str">
-        <f>E15&amp;","</f>
-        <v>{'col':'HeatingQC', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'HeatingQC', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.2">
@@ -3581,15 +3762,15 @@
         <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>'KitchenQual',</v>
+      </c>
+      <c r="P16" t="str">
         <f t="shared" si="0"/>
-        <v>'KitchenQual',</v>
-      </c>
-      <c r="P16" t="str">
-        <f>E16&amp;","</f>
-        <v>{'col':'KitchenQual', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'KitchenQual', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.2">
@@ -3597,15 +3778,15 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>135</v>
+        <v>178</v>
       </c>
       <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>'FireplaceQu',</v>
+      </c>
+      <c r="P17" t="str">
         <f t="shared" si="0"/>
-        <v>'FireplaceQu',</v>
-      </c>
-      <c r="P17" t="str">
-        <f>E17&amp;","</f>
-        <v>{'col':'FireplaceQu', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'FireplaceQu', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.2">
@@ -3613,15 +3794,15 @@
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>'GarageFinish',</v>
+      </c>
+      <c r="P18" t="str">
         <f t="shared" si="0"/>
-        <v>'GarageFinish',</v>
-      </c>
-      <c r="P18" t="str">
-        <f>E18&amp;","</f>
-        <v>{'col':'GarageFinish', mapping:{'Fin':1,'RFn':2,'Unf':3,'NA':4,}},</v>
+        <v>{'col':'GarageFinish', 'mapping':{'Fin':1,'RFn':2,'Unf':3,'NA':4,}},</v>
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.2">
@@ -3629,15 +3810,15 @@
         <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>'GarageQual',</v>
+      </c>
+      <c r="P19" t="str">
         <f t="shared" si="0"/>
-        <v>'GarageQual',</v>
-      </c>
-      <c r="P19" t="str">
-        <f>E19&amp;","</f>
-        <v>{'col':'GarageQual', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'GarageQual', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.2">
@@ -3645,15 +3826,15 @@
         <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>'GarageCond',</v>
+      </c>
+      <c r="P20" t="str">
         <f t="shared" si="0"/>
-        <v>'GarageCond',</v>
-      </c>
-      <c r="P20" t="str">
-        <f>E20&amp;","</f>
-        <v>{'col':'GarageCond', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'GarageCond', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.2">
@@ -3661,15 +3842,15 @@
         <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>'PavedDrive',</v>
+      </c>
+      <c r="P21" t="str">
         <f t="shared" si="0"/>
-        <v>'PavedDrive',</v>
-      </c>
-      <c r="P21" t="str">
-        <f>E21&amp;","</f>
-        <v>{'col':'PavedDrive', mapping:{'Y':1,'P':2,'N':3}},</v>
+        <v>{'col':'PavedDrive', 'mapping':{'Y':1,'P':2,'N':3}},</v>
       </c>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.2">
@@ -3677,28 +3858,28 @@
         <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>'PoolQC',</v>
+      </c>
+      <c r="P22" t="str">
         <f t="shared" si="0"/>
-        <v>'PoolQC',</v>
-      </c>
-      <c r="P22" t="str">
-        <f>E22&amp;","</f>
-        <v>{'col':'PoolQC', mapping:{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
+        <v>{'col':'PoolQC', 'mapping':{'NA':0,'Ex':1,'Gd':2,'TA':3,'Fa':4,'Po':5,}},</v>
       </c>
     </row>
     <row r="23" spans="4:16" x14ac:dyDescent="0.2">
       <c r="M23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="P23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="M26" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3711,7 +3892,7 @@
   <dimension ref="C3:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3721,7 +3902,7 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">

</xml_diff>